<commit_message>
Fix Excel pivot format parsing and date handling - Updated Excel parser to handle pivot-style format where columns are dates - Implemented yyyy-MM-dd internal date storage with display formatting - Fixed HoursGrid to use Date objects throughout for consistency - Added comprehensive debugging for data flow tracking - Resolved year preservation issue (2024/2025 confusion) The parser now correctly handles: - Pivot format: rows are employee-project combos, columns are week dates - Traditional format: each row is a single assignment - Date normalization to Monday of each week - Full year preservation in yyyy-MM-dd format
</commit_message>
<xml_diff>
--- a/public/ScheduleSample.xlsx
+++ b/public/ScheduleSample.xlsx
@@ -362,7 +362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
@@ -640,41 +640,42 @@
         <v>2</v>
       </c>
       <c r="D1" s="2">
-        <v>46027.0</v>
+        <v>45887.0</v>
       </c>
       <c r="E1" s="2">
-        <v>46034.0</v>
+        <v>45894.0</v>
       </c>
       <c r="F1" s="2">
-        <v>46041.0</v>
+        <v>45901.0</v>
       </c>
       <c r="G1" s="2">
-        <v>46048.0</v>
+        <v>45908.0</v>
       </c>
       <c r="H1" s="2">
-        <v>46055.0</v>
+        <v>45915.0</v>
       </c>
       <c r="I1" s="2">
-        <v>46062.0</v>
+        <v>45922.0</v>
       </c>
       <c r="J1" s="2">
-        <v>46069.0</v>
+        <v>45929.0</v>
       </c>
       <c r="K1" s="2">
-        <v>46076.0</v>
+        <v>45936.0</v>
       </c>
       <c r="L1" s="2">
-        <v>46083.0</v>
+        <v>45943.0</v>
       </c>
       <c r="M1" s="2">
-        <v>46090.0</v>
+        <v>45950.0</v>
       </c>
       <c r="N1" s="2">
-        <v>46097.0</v>
+        <v>45957.0</v>
       </c>
       <c r="O1" s="2">
-        <v>46104.0</v>
-      </c>
+        <v>45964.0</v>
+      </c>
+      <c r="P1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">

</xml_diff>